<commit_message>
phân công lần 7
</commit_message>
<xml_diff>
--- a/ProjectDocuments/Nhom11/PhanCongThanhVienNhom11.xlsx
+++ b/ProjectDocuments/Nhom11/PhanCongThanhVienNhom11.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="69">
   <si>
     <t>STT</t>
   </si>
@@ -81,19 +81,148 @@
     <t>7</t>
   </si>
   <si>
-    <t>29/4/2010</t>
-  </si>
-  <si>
-    <t>29/5/2010</t>
-  </si>
-  <si>
-    <t>25/4/2010</t>
-  </si>
-  <si>
     <t>14/4/2010</t>
   </si>
   <si>
-    <t xml:space="preserve">ghi rõ </t>
+    <t>0712187</t>
+  </si>
+  <si>
+    <t>Lý Hoài</t>
+  </si>
+  <si>
+    <t>0712188</t>
+  </si>
+  <si>
+    <t>Phan Lê Huỳnh</t>
+  </si>
+  <si>
+    <t>0712236</t>
+  </si>
+  <si>
+    <t>Phan Vũ Lâm</t>
+  </si>
+  <si>
+    <t>0712365</t>
+  </si>
+  <si>
+    <t>Nguyễn Hồ Mẫn Sáng</t>
+  </si>
+  <si>
+    <t>0712381</t>
+  </si>
+  <si>
+    <t>La Minh Tâm</t>
+  </si>
+  <si>
+    <t>thiết kế cơ sở dữ liệu lưu reading</t>
+  </si>
+  <si>
+    <t>thiết kế cơ sở dữ liệu lưu speaking</t>
+  </si>
+  <si>
+    <t>thiết kế cơ sở dữ liệu lưu listening</t>
+  </si>
+  <si>
+    <t>thiết kế cơ sở dữ liệu lưu writing</t>
+  </si>
+  <si>
+    <t>thiết kế cơ sở dữ liệu lưu language focus</t>
+  </si>
+  <si>
+    <t>bình thường</t>
+  </si>
+  <si>
+    <t>16/4/2010</t>
+  </si>
+  <si>
+    <t>30/4/2010</t>
+  </si>
+  <si>
+    <t>23/5/2010</t>
+  </si>
+  <si>
+    <t>28/5/2010</t>
+  </si>
+  <si>
+    <t>xây dựng proceduce cho  reading</t>
+  </si>
+  <si>
+    <t>xây dựng proceduce cho  speaking</t>
+  </si>
+  <si>
+    <t>xây dựng proceduce cho  listening</t>
+  </si>
+  <si>
+    <t>xây dựng proceduce cho  writing</t>
+  </si>
+  <si>
+    <t>xây dựng proceduce cho  language focus</t>
+  </si>
+  <si>
+    <t>22/4/2010</t>
+  </si>
+  <si>
+    <t>bảng mô tả cơ sở dữ liệu lưu reading</t>
+  </si>
+  <si>
+    <t>bảng mô tả cơ sở dữ liệu lưu speaking</t>
+  </si>
+  <si>
+    <t>bảng mô tả cơ sở dữ liệu lưu listening</t>
+  </si>
+  <si>
+    <t>bảng mô tả cơ sở dữ liệu lưu writing</t>
+  </si>
+  <si>
+    <t>bảng mô tả cơ sở dữ liệu lưu language focus</t>
+  </si>
+  <si>
+    <t>nhập liệu cho reading</t>
+  </si>
+  <si>
+    <t>nhập liệu cho vocabulary</t>
+  </si>
+  <si>
+    <t>20/5/2010</t>
+  </si>
+  <si>
+    <t>thiết kế giao diện</t>
+  </si>
+  <si>
+    <t>thiết kế xử lý</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>30/5/2010</t>
+  </si>
+  <si>
+    <t>control speaking task 0</t>
+  </si>
+  <si>
+    <t>control speaking task 1</t>
+  </si>
+  <si>
+    <t>quan trọng</t>
+  </si>
+  <si>
+    <t>nhập liệu speaking (unit 1-3)</t>
+  </si>
+  <si>
+    <t>nhập liệu speaking (unit 4-6)</t>
+  </si>
+  <si>
+    <t>nhập liệu speaking (unit 7-9)</t>
+  </si>
+  <si>
+    <t>nhập liệu speaking (unit 10-12)</t>
+  </si>
+  <si>
+    <t>nhập liệu speaking (unit 13-16)</t>
   </si>
 </sst>
 </file>
@@ -223,7 +352,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -239,8 +368,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -250,13 +377,24 @@
     <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="9" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
@@ -556,17 +694,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -580,7 +718,7 @@
       <c r="C1" s="6"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="17"/>
+      <c r="F1" s="15"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -634,7 +772,7 @@
       <c r="E8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="17" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="7" t="s">
@@ -647,82 +785,150 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15">
+    <row r="9" spans="1:9" ht="30">
+      <c r="A9" s="19">
+        <v>11</v>
+      </c>
+      <c r="B9" s="19">
         <v>1</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="22" t="s">
-        <v>25</v>
+      <c r="C9" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>32</v>
       </c>
       <c r="F9" s="20">
-        <v>40455</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15">
+        <v>40241</v>
+      </c>
+      <c r="G9" s="20">
+        <v>40363</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30">
+      <c r="A10" s="19">
+        <v>11</v>
+      </c>
+      <c r="B10" s="19">
         <v>2</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="C10" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>33</v>
+      </c>
       <c r="F10" s="20">
-        <v>40455</v>
-      </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15">
+        <v>40241</v>
+      </c>
+      <c r="G10" s="20">
+        <v>40363</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30">
+      <c r="A11" s="19">
+        <v>11</v>
+      </c>
+      <c r="B11" s="19">
         <v>3</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
+      <c r="C11" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>34</v>
+      </c>
       <c r="F11" s="20">
-        <v>40455</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15">
+        <v>40241</v>
+      </c>
+      <c r="G11" s="20">
+        <v>40363</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30">
+      <c r="A12" s="19">
+        <v>11</v>
+      </c>
+      <c r="B12" s="19">
         <v>4</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
+      <c r="C12" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="F12" s="20">
-        <v>40455</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15">
+        <v>40241</v>
+      </c>
+      <c r="G12" s="20">
+        <v>40363</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45">
+      <c r="A13" s="19">
+        <v>11</v>
+      </c>
+      <c r="B13" s="19">
         <v>5</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
+      <c r="C13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>36</v>
+      </c>
       <c r="F13" s="20">
-        <v>40455</v>
-      </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
+        <v>40241</v>
+      </c>
+      <c r="G13" s="20">
+        <v>40363</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="12" t="s">
@@ -749,7 +955,7 @@
       <c r="E16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="17" t="s">
         <v>4</v>
       </c>
       <c r="G16" s="7" t="s">
@@ -762,80 +968,150 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15">
+    <row r="17" spans="1:9" ht="45">
+      <c r="A17" s="19">
+        <v>11</v>
+      </c>
+      <c r="B17" s="19">
         <v>1</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="21" t="s">
+      <c r="C17" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="23">
+        <v>40425</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45">
+      <c r="A18" s="19">
+        <v>11</v>
+      </c>
+      <c r="B18" s="19">
+        <v>2</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15">
-        <v>2</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15">
+      <c r="D18" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="23">
+        <v>40425</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45">
+      <c r="A19" s="19">
+        <v>11</v>
+      </c>
+      <c r="B19" s="19">
         <v>3</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15">
+      <c r="C19" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="23">
+        <v>40425</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="45">
+      <c r="A20" s="19">
+        <v>11</v>
+      </c>
+      <c r="B20" s="19">
         <v>4</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15">
+      <c r="C20" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="23">
+        <v>40425</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="45">
+      <c r="A21" s="19">
+        <v>11</v>
+      </c>
+      <c r="B21" s="19">
         <v>5</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
+      <c r="C21" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="23">
+        <v>40425</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="12" t="s">
@@ -862,7 +1138,7 @@
       <c r="E24" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="17" t="s">
         <v>4</v>
       </c>
       <c r="G24" s="7" t="s">
@@ -875,80 +1151,150 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15">
+    <row r="25" spans="1:9" ht="45">
+      <c r="A25" s="19">
+        <v>11</v>
+      </c>
+      <c r="B25" s="19">
         <v>1</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="21" t="s">
+      <c r="C25" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15">
+      <c r="E25" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="45">
+      <c r="A26" s="19">
+        <v>11</v>
+      </c>
+      <c r="B26" s="19">
         <v>2</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15">
+      <c r="C26" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="45">
+      <c r="A27" s="19">
+        <v>11</v>
+      </c>
+      <c r="B27" s="19">
         <v>3</v>
       </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15">
+      <c r="C27" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30">
+      <c r="A28" s="19">
+        <v>11</v>
+      </c>
+      <c r="B28" s="19">
         <v>4</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15">
+      <c r="C28" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="45">
+      <c r="A29" s="19">
+        <v>11</v>
+      </c>
+      <c r="B29" s="19">
         <v>5</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
+      <c r="C29" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="12" t="s">
@@ -975,7 +1321,7 @@
       <c r="E32" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="19" t="s">
+      <c r="F32" s="17" t="s">
         <v>4</v>
       </c>
       <c r="G32" s="7" t="s">
@@ -988,80 +1334,150 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15">
+    <row r="33" spans="1:9" ht="30">
+      <c r="A33" s="19">
+        <v>11</v>
+      </c>
+      <c r="B33" s="19">
         <v>1</v>
       </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15">
+      <c r="C33" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="20">
+        <v>40364</v>
+      </c>
+      <c r="H33" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I33" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30">
+      <c r="A34" s="19">
+        <v>11</v>
+      </c>
+      <c r="B34" s="19">
         <v>2</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15">
+      <c r="C34" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="20">
+        <v>40364</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I34" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30">
+      <c r="A35" s="19">
+        <v>11</v>
+      </c>
+      <c r="B35" s="19">
         <v>3</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15">
+      <c r="C35" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="20">
+        <v>40364</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30">
+      <c r="A36" s="19">
+        <v>11</v>
+      </c>
+      <c r="B36" s="19">
         <v>4</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15">
+      <c r="C36" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" s="20">
+        <v>40364</v>
+      </c>
+      <c r="H36" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I36" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30">
+      <c r="A37" s="19">
+        <v>11</v>
+      </c>
+      <c r="B37" s="19">
         <v>5</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
+      <c r="C37" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37" s="20">
+        <v>40364</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I37" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="12" t="s">
@@ -1088,7 +1504,7 @@
       <c r="E40" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="19" t="s">
+      <c r="F40" s="17" t="s">
         <v>4</v>
       </c>
       <c r="G40" s="7" t="s">
@@ -1102,79 +1518,149 @@
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15">
+      <c r="A41" s="19">
+        <v>11</v>
+      </c>
+      <c r="B41" s="19">
         <v>1</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
+      <c r="C41" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>56</v>
+      </c>
       <c r="F41" s="20">
-        <v>40364</v>
-      </c>
-      <c r="G41" s="15"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
+        <v>40487</v>
+      </c>
+      <c r="G41" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H41" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I41" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="15"/>
-      <c r="B42" s="15">
+      <c r="A42" s="19">
+        <v>11</v>
+      </c>
+      <c r="B42" s="19">
         <v>2</v>
       </c>
-      <c r="C42" s="16"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
+      <c r="C42" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>57</v>
+      </c>
       <c r="F42" s="20">
-        <v>40364</v>
-      </c>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
+        <v>40487</v>
+      </c>
+      <c r="G42" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I42" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15">
+      <c r="A43" s="19">
+        <v>11</v>
+      </c>
+      <c r="B43" s="19">
         <v>3</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
+      <c r="C43" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>58</v>
+      </c>
       <c r="F43" s="20">
-        <v>40364</v>
-      </c>
-      <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
+        <v>40487</v>
+      </c>
+      <c r="G43" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I43" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15">
+      <c r="A44" s="19">
+        <v>11</v>
+      </c>
+      <c r="B44" s="19">
         <v>4</v>
       </c>
-      <c r="C44" s="16"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
+      <c r="C44" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>58</v>
+      </c>
       <c r="F44" s="20">
-        <v>40364</v>
-      </c>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
+        <v>40487</v>
+      </c>
+      <c r="G44" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H44" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="15"/>
-      <c r="B45" s="15">
+      <c r="A45" s="19">
+        <v>11</v>
+      </c>
+      <c r="B45" s="19">
         <v>5</v>
       </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
+      <c r="C45" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="F45" s="20">
-        <v>40364</v>
-      </c>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
+        <v>40487</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H45" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I45" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="12" t="s">
@@ -1201,7 +1687,7 @@
       <c r="E48" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F48" s="19" t="s">
+      <c r="F48" s="17" t="s">
         <v>4</v>
       </c>
       <c r="G48" s="7" t="s">
@@ -1214,80 +1700,150 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="15"/>
-      <c r="B49" s="15">
+    <row r="49" spans="1:9" ht="30">
+      <c r="A49" s="19">
+        <v>11</v>
+      </c>
+      <c r="B49" s="19">
         <v>1</v>
       </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="21" t="s">
+      <c r="C49" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="15"/>
-      <c r="B50" s="15">
+      <c r="D49" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F49" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G49" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H49" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I49" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="30">
+      <c r="A50" s="19">
+        <v>11</v>
+      </c>
+      <c r="B50" s="19">
         <v>2</v>
       </c>
-      <c r="C50" s="16"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="15"/>
-      <c r="B51" s="15">
+      <c r="C50" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F50" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G50" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H50" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I50" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="30">
+      <c r="A51" s="19">
+        <v>11</v>
+      </c>
+      <c r="B51" s="19">
         <v>3</v>
       </c>
-      <c r="C51" s="16"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="15"/>
-      <c r="B52" s="15">
+      <c r="C51" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F51" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G51" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H51" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I51" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="30">
+      <c r="A52" s="19">
+        <v>11</v>
+      </c>
+      <c r="B52" s="19">
         <v>4</v>
       </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="15"/>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="15"/>
-      <c r="B53" s="15">
+      <c r="C52" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G52" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H52" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I52" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="30">
+      <c r="A53" s="19">
+        <v>11</v>
+      </c>
+      <c r="B53" s="19">
         <v>5</v>
       </c>
-      <c r="C53" s="16"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
+      <c r="C53" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F53" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G53" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="H53" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I53" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="12" t="s">
@@ -1314,7 +1870,7 @@
       <c r="E56" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F56" s="19" t="s">
+      <c r="F56" s="17" t="s">
         <v>4</v>
       </c>
       <c r="G56" s="7" t="s">
@@ -1327,80 +1883,150 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="15"/>
-      <c r="B57" s="15">
+    <row r="57" spans="1:9" ht="30">
+      <c r="A57" s="19">
+        <v>11</v>
+      </c>
+      <c r="B57" s="19">
         <v>1</v>
       </c>
-      <c r="C57" s="16"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="20">
+      <c r="C57" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F57" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G57" s="20">
         <v>40184</v>
       </c>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15"/>
-      <c r="I57" s="15"/>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="15"/>
-      <c r="B58" s="15">
+      <c r="H57" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I57" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="30">
+      <c r="A58" s="19">
+        <v>11</v>
+      </c>
+      <c r="B58" s="19">
         <v>2</v>
       </c>
-      <c r="C58" s="16"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="20">
+      <c r="C58" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F58" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G58" s="20">
         <v>40184</v>
       </c>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="15"/>
-      <c r="B59" s="15">
+      <c r="H58" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I58" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="30">
+      <c r="A59" s="19">
+        <v>11</v>
+      </c>
+      <c r="B59" s="19">
         <v>3</v>
       </c>
-      <c r="C59" s="16"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="20">
+      <c r="C59" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F59" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G59" s="20">
         <v>40184</v>
       </c>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="15"/>
-      <c r="B60" s="15">
+      <c r="H59" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I59" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="30">
+      <c r="A60" s="19">
+        <v>11</v>
+      </c>
+      <c r="B60" s="19">
         <v>4</v>
       </c>
-      <c r="C60" s="16"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="20">
+      <c r="C60" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F60" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G60" s="20">
         <v>40184</v>
       </c>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
-      <c r="I60" s="15"/>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="15"/>
-      <c r="B61" s="15">
+      <c r="H60" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I60" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="30">
+      <c r="A61" s="19">
+        <v>11</v>
+      </c>
+      <c r="B61" s="19">
         <v>5</v>
       </c>
-      <c r="C61" s="16"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="20">
+      <c r="C61" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F61" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G61" s="20">
         <v>40184</v>
       </c>
-      <c r="G61" s="15"/>
-      <c r="H61" s="15"/>
-      <c r="I61" s="15"/>
+      <c r="H61" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I61" s="19" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>